<commit_message>
add relation values to input for jet fuel
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/jet_fuel/Model_Data_Base_jet_fuel_4_InOutputs.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/jet_fuel/Model_Data_Base_jet_fuel_4_InOutputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/jet_fuel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\jet_fuel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="13_ncr:1_{883EF14E-D4B3-4A10-B767-9D8AFEDD8A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E12126CF-13FE-4E19-80E1-4EB74A7DB5E2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D2752D-8B32-4A9E-8419-4938662763FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="-21600" windowWidth="25800" windowHeight="21000" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="125">
   <si>
     <t>Unit</t>
   </si>
@@ -367,9 +367,6 @@
     <t>Auxilliary</t>
   </si>
   <si>
-    <t>internal_heat</t>
-  </si>
-  <si>
     <t>Auxiliary</t>
   </si>
   <si>
@@ -443,6 +440,15 @@
   </si>
   <si>
     <t>minimum_op_point</t>
+  </si>
+  <si>
+    <t>diesel</t>
+  </si>
+  <si>
+    <t>power_steam</t>
+  </si>
+  <si>
+    <t>heat_recovery</t>
   </si>
 </sst>
 </file>
@@ -484,7 +490,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -536,11 +542,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -552,19 +567,225 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="19">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -614,8 +835,8 @@
     <tableColumn id="13" xr3:uid="{6AD6D1D4-6C5C-4CAB-BFAA-59566A4C5F83}" name="fom_cost"/>
     <tableColumn id="23" xr3:uid="{8D12B570-57AA-4CE8-8346-92640B0E4FE4}" name="vom_cost"/>
     <tableColumn id="7" xr3:uid="{8B684245-CB0B-4E58-917D-96D57CE2B5AF}" name="minimum_op_point"/>
-    <tableColumn id="15" xr3:uid="{0C029686-E14C-4BAF-8B3D-3ED880CBB758}" name="resolution_output" dataDxfId="3"/>
-    <tableColumn id="16" xr3:uid="{4F32D3CC-D65E-436B-A8EE-58FBC117DA41}" name="demand" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{0C029686-E14C-4BAF-8B3D-3ED880CBB758}" name="resolution_output" dataDxfId="18"/>
+    <tableColumn id="16" xr3:uid="{4F32D3CC-D65E-436B-A8EE-58FBC117DA41}" name="demand" dataDxfId="17"/>
     <tableColumn id="19" xr3:uid="{E4B02BA0-A154-4F00-855E-6FD9D2CD7958}" name="initial_units_on"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -623,26 +844,26 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{12FAA58E-4414-4B31-B756-3FD9A04CACB5}" name="Table16" displayName="Table16" ref="A1:Q13" totalsRowShown="0">
-  <autoFilter ref="A1:Q13" xr:uid="{0333CFC6-D067-4B12-B0A1-83E429D32CCD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{12FAA58E-4414-4B31-B756-3FD9A04CACB5}" name="Table16" displayName="Table16" ref="A1:Q14" totalsRowShown="0">
+  <autoFilter ref="A1:Q14" xr:uid="{0333CFC6-D067-4B12-B0A1-83E429D32CCD}"/>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{CD5761E6-0259-4D3B-B945-2F2B9275A761}" name="Unit"/>
     <tableColumn id="2" xr3:uid="{8206E937-98CA-48B8-8ECF-A8CC8CEA0E7A}" name="Object_type"/>
-    <tableColumn id="3" xr3:uid="{25658B53-E729-4F77-A87A-2C1AA31D180F}" name="Input1"/>
-    <tableColumn id="4" xr3:uid="{C20E16FC-DEE5-46FF-98E7-EC2B1178D89F}" name="Input2"/>
-    <tableColumn id="13" xr3:uid="{C4257F9B-BEBE-4928-A299-FA13BAF91F57}" name="Input3"/>
-    <tableColumn id="14" xr3:uid="{E33FDA0D-66C9-4616-8A81-6F5E0E166ED4}" name="Input4"/>
-    <tableColumn id="5" xr3:uid="{901F195D-0BA8-4EDC-88F0-75A5DF763740}" name="Output1"/>
-    <tableColumn id="6" xr3:uid="{0D5DCA48-4EAB-497A-B34F-5091694CCF48}" name="Output2"/>
-    <tableColumn id="15" xr3:uid="{E758FC30-F120-4234-A984-DD9BB9F5CBE5}" name="Output3"/>
-    <tableColumn id="16" xr3:uid="{85570B5D-60DB-4C61-80EB-881EDB346388}" name="Output4"/>
-    <tableColumn id="10" xr3:uid="{40961C24-C288-48FE-96C9-C696058F1146}" name="Relation_In1_In2"/>
-    <tableColumn id="7" xr3:uid="{E93572D0-6388-4D7C-A2BF-3805225F4F50}" name="Relation_In1_In22"/>
-    <tableColumn id="8" xr3:uid="{BAF59A78-842A-475C-B900-52E45F0F2C02}" name="Relation_In1_In23"/>
-    <tableColumn id="11" xr3:uid="{63A0B53D-07BC-4C95-B97C-243557E4A128}" name="Relation_In_Out"/>
-    <tableColumn id="25" xr3:uid="{44B35FDD-04C5-401A-9765-766FCD023027}" name="Relation_Out1_Out2"/>
-    <tableColumn id="9" xr3:uid="{3E00680F-559F-4DED-989F-C435D3C0AEC7}" name="Relation_Out1_Out22"/>
-    <tableColumn id="12" xr3:uid="{17E13652-ACBE-480B-A89B-1AB97BFEAE60}" name="Relation_Out1_Out23"/>
+    <tableColumn id="3" xr3:uid="{25658B53-E729-4F77-A87A-2C1AA31D180F}" name="Input1" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{C20E16FC-DEE5-46FF-98E7-EC2B1178D89F}" name="Input2" dataDxfId="13"/>
+    <tableColumn id="13" xr3:uid="{C4257F9B-BEBE-4928-A299-FA13BAF91F57}" name="Input3" dataDxfId="12"/>
+    <tableColumn id="14" xr3:uid="{E33FDA0D-66C9-4616-8A81-6F5E0E166ED4}" name="Input4" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{901F195D-0BA8-4EDC-88F0-75A5DF763740}" name="Output1" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{0D5DCA48-4EAB-497A-B34F-5091694CCF48}" name="Output2" dataDxfId="9"/>
+    <tableColumn id="15" xr3:uid="{E758FC30-F120-4234-A984-DD9BB9F5CBE5}" name="Output3" dataDxfId="8"/>
+    <tableColumn id="16" xr3:uid="{85570B5D-60DB-4C61-80EB-881EDB346388}" name="Output4" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{40961C24-C288-48FE-96C9-C696058F1146}" name="Relation_In1_In2" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{E93572D0-6388-4D7C-A2BF-3805225F4F50}" name="Relation_In1_In22" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{BAF59A78-842A-475C-B900-52E45F0F2C02}" name="Relation_In1_In23" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{63A0B53D-07BC-4C95-B97C-243557E4A128}" name="Relation_In_Out" dataDxfId="3"/>
+    <tableColumn id="25" xr3:uid="{44B35FDD-04C5-401A-9765-766FCD023027}" name="Relation_Out1_Out2" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{3E00680F-559F-4DED-989F-C435D3C0AEC7}" name="Relation_Out1_Out22" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{17E13652-ACBE-480B-A89B-1AB97BFEAE60}" name="Relation_Out1_Out23" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -657,7 +878,7 @@
     <tableColumn id="3" xr3:uid="{BC9D86F7-8FDE-4FAF-A6B2-8BF7829723EF}" name="Input1"/>
     <tableColumn id="4" xr3:uid="{31F6D71E-306D-4146-A535-A6A629EBE2DC}" name="Input2"/>
     <tableColumn id="5" xr3:uid="{E176ABAF-D150-4E6A-8921-E24FCEB64CEB}" name="Output1"/>
-    <tableColumn id="22" xr3:uid="{EB53F534-595A-4E1E-82EE-E811ECDB4974}" name="Output2" dataDxfId="1"/>
+    <tableColumn id="22" xr3:uid="{EB53F534-595A-4E1E-82EE-E811ECDB4974}" name="Output2" dataDxfId="16"/>
     <tableColumn id="6" xr3:uid="{C9818184-D13F-4AF4-AE3A-C64F072A0385}" name="Connection_type"/>
     <tableColumn id="15" xr3:uid="{52C8ADC6-49B2-4339-A761-5E82E904E3A6}" name="Cap_Input1_existing"/>
     <tableColumn id="14" xr3:uid="{F6461E15-EE92-48B4-8879-9BDE3EBAAA17}" name="Cap_Input1_max"/>
@@ -688,7 +909,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}" name="Table134" displayName="Table134" ref="A1:K5" totalsRowShown="0">
   <autoFilter ref="A1:K5" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="15"/>
     <tableColumn id="4" xr3:uid="{AEAA1B51-84C1-491F-81D5-7757B30BDCCD}" name="Object_type"/>
     <tableColumn id="6" xr3:uid="{FA5F8582-61FC-4A96-9E8D-E08E92F1962D}" name="value_before"/>
     <tableColumn id="2" xr3:uid="{1FB70133-79C8-41A8-BCD5-AC8AA5856E5B}" name="has_state"/>
@@ -1016,7 +1237,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:T13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1032,7 +1255,7 @@
         <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D1" t="s">
         <v>37</v>
@@ -1041,16 +1264,16 @@
         <v>33</v>
       </c>
       <c r="F1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" t="s">
         <v>118</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>119</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>120</v>
-      </c>
-      <c r="I1" t="s">
-        <v>121</v>
       </c>
       <c r="J1" t="s">
         <v>88</v>
@@ -1068,7 +1291,7 @@
         <v>27</v>
       </c>
       <c r="O1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P1" t="s">
         <v>39</v>
@@ -1095,10 +1318,10 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" t="s">
         <v>99</v>
-      </c>
-      <c r="B3" t="s">
-        <v>100</v>
       </c>
       <c r="C3" t="s">
         <v>64</v>
@@ -1108,10 +1331,10 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" t="s">
         <v>101</v>
-      </c>
-      <c r="B4" t="s">
-        <v>102</v>
       </c>
       <c r="C4" t="s">
         <v>64</v>
@@ -1227,7 +1450,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>96</v>
@@ -1242,32 +1465,20 @@
       <c r="Q12" s="1"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="B13" s="9" t="s">
+      <c r="A13" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
       <c r="N13">
         <v>26.81</v>
       </c>
-      <c r="O13" s="10"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="10"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1285,9 +1496,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8478C130-C296-4571-ABF4-62E91E9E2767}">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1309,10 +1522,10 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" t="s">
         <v>113</v>
-      </c>
-      <c r="F1" t="s">
-        <v>114</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -1321,268 +1534,440 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
+        <v>114</v>
+      </c>
+      <c r="J1" t="s">
         <v>115</v>
       </c>
-      <c r="J1" t="s">
-        <v>116</v>
-      </c>
       <c r="K1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L1" t="s">
         <v>110</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>111</v>
-      </c>
-      <c r="M1" t="s">
-        <v>112</v>
       </c>
       <c r="N1" t="s">
         <v>16</v>
       </c>
       <c r="O1" t="s">
+        <v>106</v>
+      </c>
+      <c r="P1" t="s">
         <v>107</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>108</v>
       </c>
-      <c r="Q1" t="s">
-        <v>109</v>
-      </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G2" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
         <v>64</v>
       </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3" t="s">
         <v>64</v>
       </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" t="s">
         <v>101</v>
       </c>
-      <c r="B4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
         <v>64</v>
       </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G5" t="s">
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="K5">
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3">
         <v>5.8500000000000002E-3</v>
       </c>
-      <c r="O5">
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3">
         <v>1.76</v>
       </c>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G6" t="s">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="K6">
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2">
         <v>3.529412E-3</v>
       </c>
-      <c r="N6">
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2">
         <v>3.529412E-3</v>
       </c>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>71</v>
+      <c r="A7" t="s">
+        <v>76</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D7" t="s">
-        <v>70</v>
-      </c>
-      <c r="G7" t="s">
-        <v>72</v>
-      </c>
-      <c r="H7" t="s">
-        <v>66</v>
-      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3">
+        <v>161.1904761904762</v>
+      </c>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3">
+        <v>2</v>
+      </c>
+      <c r="O7" s="3">
+        <v>1</v>
+      </c>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2">
+        <v>2.8982576753129519</v>
+      </c>
+      <c r="L8" s="2">
+        <v>12.285714285714285</v>
+      </c>
+      <c r="M8" s="2">
+        <v>3.0714285714285712</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0.86</v>
+      </c>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>90</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>43</v>
       </c>
-      <c r="C8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C9" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G8" t="s">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K8">
-        <v>7.2437800000000002E-4</v>
-      </c>
-      <c r="N8">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" t="s">
-        <v>75</v>
-      </c>
-      <c r="H9" t="s">
-        <v>94</v>
-      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3">
+        <v>9.8530247749999979E-4</v>
+      </c>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3">
+        <v>1.0101010101010102</v>
+      </c>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
-        <v>76</v>
+      <c r="A10" t="s">
+        <v>102</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" t="s">
-        <v>73</v>
-      </c>
-      <c r="G10" t="s">
-        <v>79</v>
-      </c>
-      <c r="H10" t="s">
-        <v>78</v>
+        <v>96</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B11" t="s">
         <v>96</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3">
+        <v>1</v>
+      </c>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="G11" t="s">
-        <v>97</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="J12" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="O11">
-        <v>0.4</v>
-      </c>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B12" s="2" t="s">
+      <c r="K12" s="10">
+        <v>42.75</v>
+      </c>
+      <c r="L12" s="10">
+        <v>1.6132075471698113</v>
+      </c>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10">
+        <v>1.6285714285714283</v>
+      </c>
+      <c r="O12" s="10">
+        <v>6.7340067340067344</v>
+      </c>
+      <c r="P12" s="10">
+        <v>5.5096418732782366</v>
+      </c>
+      <c r="Q12" s="10"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="B13" s="9" t="s">
+      <c r="C13" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3">
+        <v>1.1883541295306002</v>
+      </c>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
+      <c r="C14" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10">
+        <v>1</v>
+      </c>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P11" xr:uid="{47312732-C7F3-4B68-A90F-B132C94369E6}">
-      <formula1>"h, D, W, M, Q, Y"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2119,7 +2504,7 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>